<commit_message>
for the report of July
</commit_message>
<xml_diff>
--- a/tables/2021-07/sup_table_overview_Jul.xlsx
+++ b/tables/2021-07/sup_table_overview_Jul.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="241">
   <si>
     <t>Population size</t>
   </si>
@@ -176,103 +176,103 @@
     <t>TI</t>
   </si>
   <si>
-    <t>1.17 (1.08-1.27)</t>
-  </si>
-  <si>
-    <t>1.28 (1.02-1.58)</t>
-  </si>
-  <si>
-    <t>1.52 (1.35-1.68)</t>
-  </si>
-  <si>
-    <t>1.32 (0.88-1.90)</t>
-  </si>
-  <si>
-    <t>1.31 (1.13-1.51)</t>
-  </si>
-  <si>
-    <t>1.12 (0.88-1.40)</t>
-  </si>
-  <si>
-    <t>1.32 (0.98-1.81)</t>
-  </si>
-  <si>
-    <t>1.29 (1.11-1.50)</t>
-  </si>
-  <si>
-    <t>1.43 (0.98-1.91)</t>
-  </si>
-  <si>
-    <t>1.30 (0.55-2.37)</t>
-  </si>
-  <si>
-    <t>1.33 (1.02-1.63)</t>
-  </si>
-  <si>
-    <t>1.25 (1.01-1.53)</t>
-  </si>
-  <si>
-    <t>1.34 (1.04-1.69)</t>
-  </si>
-  <si>
-    <t>1.36 (1.10-1.65)</t>
-  </si>
-  <si>
-    <t>1.42 (0.98-1.95)</t>
-  </si>
-  <si>
-    <t>1.25 (0.66-1.94)</t>
-  </si>
-  <si>
-    <t>1.37 (1.05-1.68)</t>
-  </si>
-  <si>
-    <t>1.22 (0.58-2.07)</t>
-  </si>
-  <si>
-    <t>1.35 (0.59-2.66)</t>
-  </si>
-  <si>
-    <t>1.07 (0.78-1.41)</t>
-  </si>
-  <si>
-    <t>1.64 (0.32-4.37)</t>
-  </si>
-  <si>
-    <t>1.07 (0.75-1.44)</t>
-  </si>
-  <si>
-    <t>1.23 (0.74-1.99)</t>
-  </si>
-  <si>
-    <t>1.59 (0.00-11.29)</t>
-  </si>
-  <si>
-    <t>1.08 (0.26-2.50)</t>
-  </si>
-  <si>
-    <t>1.39 (0.73-2.11)</t>
-  </si>
-  <si>
-    <t>1.15 (0.93-1.38)</t>
-  </si>
-  <si>
-    <t>1.27 (0.71-2.05)</t>
-  </si>
-  <si>
-    <t>1.31 (0.94-1.80)</t>
-  </si>
-  <si>
-    <t>1.23 (1.07-1.39)</t>
-  </si>
-  <si>
-    <t>1.15 (0.87-1.53)</t>
-  </si>
-  <si>
-    <t>1.18 (0.81-1.60)</t>
-  </si>
-  <si>
-    <t>1.14 (0.90-1.41)</t>
+    <t>1.22 (1.09-1.35)</t>
+  </si>
+  <si>
+    <t>1.23 (0.98-1.56)</t>
+  </si>
+  <si>
+    <t>1.34 (1.21-1.48)</t>
+  </si>
+  <si>
+    <t>1.25 (0.89-1.81)</t>
+  </si>
+  <si>
+    <t>1.29 (1.11-1.46)</t>
+  </si>
+  <si>
+    <t>1.08 (0.84-1.34)</t>
+  </si>
+  <si>
+    <t>1.41 (1.00-1.84)</t>
+  </si>
+  <si>
+    <t>1.36 (1.14-1.58)</t>
+  </si>
+  <si>
+    <t>1.48 (0.99-1.84)</t>
+  </si>
+  <si>
+    <t>1.41 (0.61-2.28)</t>
+  </si>
+  <si>
+    <t>1.33 (1.04-1.62)</t>
+  </si>
+  <si>
+    <t>1.26 (1.02-1.53)</t>
+  </si>
+  <si>
+    <t>1.29 (1.04-1.58)</t>
+  </si>
+  <si>
+    <t>1.35 (1.08-1.64)</t>
+  </si>
+  <si>
+    <t>1.38 (0.99-1.81)</t>
+  </si>
+  <si>
+    <t>1.20 (0.66-1.91)</t>
+  </si>
+  <si>
+    <t>1.27 (1.01-1.50)</t>
+  </si>
+  <si>
+    <t>1.15 (0.55-1.98)</t>
+  </si>
+  <si>
+    <t>1.33 (0.61-2.56)</t>
+  </si>
+  <si>
+    <t>1.10 (0.80-1.45)</t>
+  </si>
+  <si>
+    <t>1.58 (0.34-3.81)</t>
+  </si>
+  <si>
+    <t>1.04 (0.74-1.42)</t>
+  </si>
+  <si>
+    <t>1.23 (0.75-1.92)</t>
+  </si>
+  <si>
+    <t>1.27 (0.00-11.03)</t>
+  </si>
+  <si>
+    <t>1.14 (0.32-2.54)</t>
+  </si>
+  <si>
+    <t>1.31 (0.72-1.97)</t>
+  </si>
+  <si>
+    <t>1.18 (0.96-1.41)</t>
+  </si>
+  <si>
+    <t>1.31 (0.71-2.02)</t>
+  </si>
+  <si>
+    <t>1.33 (0.95-1.81)</t>
+  </si>
+  <si>
+    <t>1.12 (0.99-1.27)</t>
+  </si>
+  <si>
+    <t>1.13 (0.86-1.50)</t>
+  </si>
+  <si>
+    <t>1.15 (0.82-1.57)</t>
+  </si>
+  <si>
+    <t>1.11 (0.89-1.37)</t>
   </si>
   <si>
     <t>2.42</t>
@@ -284,13 +284,13 @@
     <t>4.12</t>
   </si>
   <si>
-    <t>1.67</t>
+    <t>1.68</t>
   </si>
   <si>
     <t>1.71</t>
   </si>
   <si>
-    <t>2.62</t>
+    <t>2.63</t>
   </si>
   <si>
     <t>1.69</t>
@@ -311,52 +311,55 @@
     <t>1.50</t>
   </si>
   <si>
-    <t>2.12</t>
+    <t>2.13</t>
   </si>
   <si>
     <t>1.29</t>
   </si>
   <si>
+    <t>2.93</t>
+  </si>
+  <si>
+    <t>4.14</t>
+  </si>
+  <si>
+    <t>2.06</t>
+  </si>
+  <si>
+    <t>2.51</t>
+  </si>
+  <si>
+    <t>3.86</t>
+  </si>
+  <si>
+    <t>0.43</t>
+  </si>
+  <si>
+    <t>1.95</t>
+  </si>
+  <si>
+    <t>2.84</t>
+  </si>
+  <si>
+    <t>1.28</t>
+  </si>
+  <si>
+    <t>1.20</t>
+  </si>
+  <si>
+    <t>4.08</t>
+  </si>
+  <si>
     <t>2.92</t>
   </si>
   <si>
-    <t>4.14</t>
-  </si>
-  <si>
-    <t>2.06</t>
-  </si>
-  <si>
-    <t>2.51</t>
-  </si>
-  <si>
-    <t>3.85</t>
-  </si>
-  <si>
-    <t>0.43</t>
-  </si>
-  <si>
-    <t>1.96</t>
-  </si>
-  <si>
-    <t>2.83</t>
-  </si>
-  <si>
-    <t>1.28</t>
-  </si>
-  <si>
-    <t>1.20</t>
-  </si>
-  <si>
-    <t>4.08</t>
-  </si>
-  <si>
     <t>2.11</t>
   </si>
   <si>
     <t>2.09</t>
   </si>
   <si>
-    <t>2.94</t>
+    <t>2.95</t>
   </si>
   <si>
     <t>4.18</t>
@@ -368,22 +371,22 @@
     <t>4.48</t>
   </si>
   <si>
-    <t>24.9</t>
-  </si>
-  <si>
-    <t>35.3</t>
-  </si>
-  <si>
-    <t>45.1</t>
+    <t>23.6</t>
+  </si>
+  <si>
+    <t>31.2</t>
+  </si>
+  <si>
+    <t>37.2</t>
   </si>
   <si>
     <t>4.0</t>
   </si>
   <si>
-    <t>32.5</t>
-  </si>
-  <si>
-    <t>14.8</t>
+    <t>32.1</t>
+  </si>
+  <si>
+    <t>14.6</t>
   </si>
   <si>
     <t>15.8</t>
@@ -404,7 +407,7 @@
     <t>14.0</t>
   </si>
   <si>
-    <t>53.5</t>
+    <t>53.6</t>
   </si>
   <si>
     <t>41.6</t>
@@ -425,10 +428,10 @@
     <t>4.8</t>
   </si>
   <si>
-    <t>12.7</t>
-  </si>
-  <si>
-    <t>2.4</t>
+    <t>12.6</t>
+  </si>
+  <si>
+    <t>2.5</t>
   </si>
   <si>
     <t>17.0</t>
@@ -458,22 +461,22 @@
     <t>34.7</t>
   </si>
   <si>
-    <t>3.8 (3.2-4.4)</t>
-  </si>
-  <si>
-    <t>4.6 (3.7-5.7)</t>
-  </si>
-  <si>
-    <t>2.1 (1.3-3.1)</t>
+    <t>4.0 (3.4-4.7)</t>
+  </si>
+  <si>
+    <t>5.2 (4.1-6.5)</t>
+  </si>
+  <si>
+    <t>2.5 (1.6-3.8)</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>7.4 (5.2-10.0)</t>
-  </si>
-  <si>
-    <t>21.7 (13.4-32.1)</t>
+    <t>7.4 (5.3-10.1)</t>
+  </si>
+  <si>
+    <t>22.0 (13.6-32.5)</t>
   </si>
   <si>
     <t>0.8 (0.1-2.9)</t>
@@ -542,13 +545,13 @@
     <t>1.8 (0.0-9.7)</t>
   </si>
   <si>
-    <t>0.6 (0.4-1.0)</t>
-  </si>
-  <si>
-    <t>0.6 (0.3-1.1)</t>
-  </si>
-  <si>
-    <t>0.4 (0.1-0.9)</t>
+    <t>0.7 (0.4-1.0)</t>
+  </si>
+  <si>
+    <t>0.7 (0.3-1.2)</t>
+  </si>
+  <si>
+    <t>0.4 (0.1-1.1)</t>
   </si>
   <si>
     <t>1.2 (0.4-2.6)</t>
@@ -578,22 +581,22 @@
     <t>0.4 (0.0-2.4)</t>
   </si>
   <si>
-    <t>93.3 (92.5-94.1)</t>
-  </si>
-  <si>
-    <t>93.0 (91.7-94.2)</t>
-  </si>
-  <si>
-    <t>96.6 (95.4-97.6)</t>
+    <t>93.0 (92.1-93.7)</t>
+  </si>
+  <si>
+    <t>92.1 (90.6-93.4)</t>
+  </si>
+  <si>
+    <t>95.9 (94.4-97.1)</t>
   </si>
   <si>
     <t>100.0 (69.2-100.0)</t>
   </si>
   <si>
-    <t>88.1 (84.9-90.8)</t>
-  </si>
-  <si>
-    <t>74.7 (64.0-83.6)</t>
+    <t>88.0 (84.8-90.7)</t>
+  </si>
+  <si>
+    <t>74.4 (63.6-83.4)</t>
   </si>
   <si>
     <t>95.1 (91.5-97.4)</t>
@@ -662,16 +665,16 @@
     <t>90.8 (86.3-94.2)</t>
   </si>
   <si>
-    <t>0.4 (0.3-0.7)</t>
-  </si>
-  <si>
-    <t>0.2 (0.1-0.6)</t>
+    <t>0.5 (0.3-0.7)</t>
+  </si>
+  <si>
+    <t>0.3 (0.1-0.7)</t>
   </si>
   <si>
     <t>0.6 (0.1-1.7)</t>
   </si>
   <si>
-    <t>1.2 (0.0-6.5)</t>
+    <t>1.2 (0.0-6.6)</t>
   </si>
   <si>
     <t>2.9 (1.2-5.8)</t>
@@ -689,19 +692,19 @@
     <t>0.1 (0.0-0.8)</t>
   </si>
   <si>
-    <t>1.8 (1.4-2.2)</t>
-  </si>
-  <si>
-    <t>1.5 (1.0-2.2)</t>
-  </si>
-  <si>
-    <t>0.9 (0.4-1.7)</t>
-  </si>
-  <si>
-    <t>2.8 (1.5-4.6)</t>
-  </si>
-  <si>
-    <t>2.4 (0.3-8.4)</t>
+    <t>1.9 (1.5-2.4)</t>
+  </si>
+  <si>
+    <t>1.7 (1.1-2.5)</t>
+  </si>
+  <si>
+    <t>1.1 (0.5-2.0)</t>
+  </si>
+  <si>
+    <t>2.8 (1.5-4.7)</t>
+  </si>
+  <si>
+    <t>2.4 (0.3-8.5)</t>
   </si>
   <si>
     <t>1.2 (0.3-3.6)</t>
@@ -856,7 +859,7 @@
         <v>8606033.0</v>
       </c>
       <c r="C2" t="n">
-        <v>16072.0</v>
+        <v>16085.0</v>
       </c>
       <c r="D2" t="n">
         <v>414.0</v>
@@ -865,55 +868,55 @@
         <v>54</v>
       </c>
       <c r="F2" t="n">
-        <v>774626.0</v>
+        <v>774496.0</v>
       </c>
       <c r="G2" t="n">
-        <v>9001.0</v>
+        <v>8999.0</v>
       </c>
       <c r="H2" t="s">
         <v>87</v>
       </c>
       <c r="I2" t="n">
-        <v>4001.0</v>
+        <v>3790.0</v>
       </c>
       <c r="J2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K2" t="n">
         <v>151.0</v>
       </c>
       <c r="L2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="M2" t="n">
         <v>1.0</v>
       </c>
       <c r="N2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="O2" t="n">
         <v>26.0</v>
       </c>
       <c r="P2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="Q2" t="n">
-        <v>3734.0</v>
+        <v>3523.0</v>
       </c>
       <c r="R2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="S2" t="n">
         <v>18.0</v>
       </c>
       <c r="T2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="U2" t="n">
         <v>71.0</v>
       </c>
       <c r="V2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3">
@@ -924,64 +927,64 @@
         <v>1831247.0</v>
       </c>
       <c r="C3" t="n">
-        <v>4778.0</v>
+        <v>4790.0</v>
       </c>
       <c r="D3" t="n">
-        <v>118.0</v>
+        <v>579.0</v>
       </c>
       <c r="E3" t="s">
         <v>55</v>
       </c>
       <c r="F3" t="n">
-        <v>224176.0</v>
+        <v>224195.0</v>
       </c>
       <c r="G3" t="n">
-        <v>12242.0</v>
+        <v>12243.0</v>
       </c>
       <c r="H3" t="s">
         <v>88</v>
       </c>
       <c r="I3" t="n">
-        <v>1689.0</v>
+        <v>1494.0</v>
       </c>
       <c r="J3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K3" t="n">
         <v>78.0</v>
       </c>
       <c r="L3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="M3" t="n">
         <v>0.0</v>
       </c>
       <c r="N3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O3" t="n">
         <v>10.0</v>
       </c>
       <c r="P3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Q3" t="n">
-        <v>1571.0</v>
+        <v>1376.0</v>
       </c>
       <c r="R3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="S3" t="n">
         <v>4.0</v>
       </c>
       <c r="T3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="U3" t="n">
         <v>26.0</v>
       </c>
       <c r="V3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4">
@@ -992,16 +995,16 @@
         <v>504128.0</v>
       </c>
       <c r="C4" t="n">
-        <v>2421.0</v>
+        <v>2423.0</v>
       </c>
       <c r="D4" t="n">
-        <v>1063.0</v>
+        <v>1064.0</v>
       </c>
       <c r="E4" t="s">
         <v>56</v>
       </c>
       <c r="F4" t="n">
-        <v>70814.0</v>
+        <v>70816.0</v>
       </c>
       <c r="G4" t="n">
         <v>14047.0</v>
@@ -1010,46 +1013,46 @@
         <v>89</v>
       </c>
       <c r="I4" t="n">
-        <v>1093.0</v>
+        <v>902.0</v>
       </c>
       <c r="J4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K4" t="n">
         <v>23.0</v>
       </c>
       <c r="L4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="M4" t="n">
         <v>0.0</v>
       </c>
       <c r="N4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O4" t="n">
         <v>4.0</v>
       </c>
       <c r="P4" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="Q4" t="n">
-        <v>1056.0</v>
+        <v>865.0</v>
       </c>
       <c r="R4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="S4" t="n">
         <v>0.0</v>
       </c>
       <c r="T4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U4" t="n">
         <v>10.0</v>
       </c>
       <c r="V4" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5">
@@ -1069,7 +1072,7 @@
         <v>57</v>
       </c>
       <c r="F5" t="n">
-        <v>17017.0</v>
+        <v>17018.0</v>
       </c>
       <c r="G5" t="n">
         <v>9642.0</v>
@@ -1081,43 +1084,43 @@
         <v>10.0</v>
       </c>
       <c r="J5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K5" t="n">
         <v>0.0</v>
       </c>
       <c r="L5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M5" t="n">
         <v>0.0</v>
       </c>
       <c r="N5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O5" t="n">
         <v>0.0</v>
       </c>
       <c r="P5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q5" t="n">
         <v>10.0</v>
       </c>
       <c r="R5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="S5" t="n">
         <v>0.0</v>
       </c>
       <c r="T5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U5" t="n">
         <v>0.0</v>
       </c>
       <c r="V5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6">
@@ -1128,16 +1131,16 @@
         <v>805098.0</v>
       </c>
       <c r="C6" t="n">
-        <v>1550.0</v>
+        <v>1560.0</v>
       </c>
       <c r="D6" t="n">
-        <v>426.0</v>
+        <v>429.0</v>
       </c>
       <c r="E6" t="s">
         <v>58</v>
       </c>
       <c r="F6" t="n">
-        <v>111736.0</v>
+        <v>111740.0</v>
       </c>
       <c r="G6" t="n">
         <v>13879.0</v>
@@ -1146,46 +1149,46 @@
         <v>91</v>
       </c>
       <c r="I6" t="n">
-        <v>503.0</v>
+        <v>500.0</v>
       </c>
       <c r="J6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K6" t="n">
         <v>37.0</v>
       </c>
       <c r="L6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="M6" t="n">
         <v>0.0</v>
       </c>
       <c r="N6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O6" t="n">
         <v>6.0</v>
       </c>
       <c r="P6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="Q6" t="n">
-        <v>443.0</v>
+        <v>440.0</v>
       </c>
       <c r="R6" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="S6" t="n">
         <v>3.0</v>
       </c>
       <c r="T6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="U6" t="n">
         <v>14.0</v>
       </c>
       <c r="V6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7">
@@ -1205,55 +1208,55 @@
         <v>59</v>
       </c>
       <c r="F7" t="n">
-        <v>24609.0</v>
+        <v>24621.0</v>
       </c>
       <c r="G7" t="n">
-        <v>7122.0</v>
+        <v>7126.0</v>
       </c>
       <c r="H7" t="s">
         <v>92</v>
       </c>
       <c r="I7" t="n">
-        <v>83.0</v>
+        <v>82.0</v>
       </c>
       <c r="J7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="K7" t="n">
         <v>18.0</v>
       </c>
       <c r="L7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M7" t="n">
         <v>0.0</v>
       </c>
       <c r="N7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O7" t="n">
         <v>0.0</v>
       </c>
       <c r="P7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q7" t="n">
-        <v>62.0</v>
+        <v>61.0</v>
       </c>
       <c r="R7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="S7" t="n">
         <v>1.0</v>
       </c>
       <c r="T7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="U7" t="n">
         <v>2.0</v>
       </c>
       <c r="V7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8">
@@ -1264,19 +1267,19 @@
         <v>1434841.0</v>
       </c>
       <c r="C8" t="n">
-        <v>1537.0</v>
+        <v>1538.0</v>
       </c>
       <c r="D8" t="n">
-        <v>48.0</v>
+        <v>237.0</v>
       </c>
       <c r="E8" t="s">
         <v>60</v>
       </c>
       <c r="F8" t="n">
-        <v>100188.0</v>
+        <v>100242.0</v>
       </c>
       <c r="G8" t="n">
-        <v>6983.0</v>
+        <v>6986.0</v>
       </c>
       <c r="H8" t="s">
         <v>93</v>
@@ -1285,43 +1288,43 @@
         <v>243.0</v>
       </c>
       <c r="J8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K8" t="n">
         <v>2.0</v>
       </c>
       <c r="L8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M8" t="n">
         <v>0.0</v>
       </c>
       <c r="N8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O8" t="n">
         <v>0.0</v>
       </c>
       <c r="P8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q8" t="n">
         <v>231.0</v>
       </c>
       <c r="R8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="S8" t="n">
         <v>7.0</v>
       </c>
       <c r="T8" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="U8" t="n">
         <v>3.0</v>
       </c>
       <c r="V8" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9">
@@ -1332,7 +1335,7 @@
         <v>1039474.0</v>
       </c>
       <c r="C9" t="n">
-        <v>1136.0</v>
+        <v>1137.0</v>
       </c>
       <c r="D9" t="n">
         <v>242.0</v>
@@ -1341,10 +1344,10 @@
         <v>61</v>
       </c>
       <c r="F9" t="n">
-        <v>64952.0</v>
+        <v>65005.0</v>
       </c>
       <c r="G9" t="n">
-        <v>6249.0</v>
+        <v>6254.0</v>
       </c>
       <c r="H9" t="s">
         <v>94</v>
@@ -1353,43 +1356,43 @@
         <v>231.0</v>
       </c>
       <c r="J9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K9" t="n">
         <v>2.0</v>
       </c>
       <c r="L9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="M9" t="n">
         <v>0.0</v>
       </c>
       <c r="N9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O9" t="n">
         <v>0.0</v>
       </c>
       <c r="P9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q9" t="n">
         <v>219.0</v>
       </c>
       <c r="R9" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="S9" t="n">
         <v>7.0</v>
       </c>
       <c r="T9" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="U9" t="n">
         <v>3.0</v>
       </c>
       <c r="V9" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10">
@@ -1409,7 +1412,7 @@
         <v>62</v>
       </c>
       <c r="F10" t="n">
-        <v>32782.0</v>
+        <v>32783.0</v>
       </c>
       <c r="G10" t="n">
         <v>10188.0</v>
@@ -1421,43 +1424,43 @@
         <v>2.0</v>
       </c>
       <c r="J10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K10" t="n">
         <v>0.0</v>
       </c>
       <c r="L10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M10" t="n">
         <v>0.0</v>
       </c>
       <c r="N10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O10" t="n">
         <v>0.0</v>
       </c>
       <c r="P10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q10" t="n">
         <v>2.0</v>
       </c>
       <c r="R10" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="S10" t="n">
         <v>0.0</v>
       </c>
       <c r="T10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U10" t="n">
         <v>0.0</v>
       </c>
       <c r="V10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11">
@@ -1489,43 +1492,43 @@
         <v>10.0</v>
       </c>
       <c r="J11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K11" t="n">
         <v>0.0</v>
       </c>
       <c r="L11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M11" t="n">
         <v>0.0</v>
       </c>
       <c r="N11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O11" t="n">
         <v>0.0</v>
       </c>
       <c r="P11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q11" t="n">
         <v>10.0</v>
       </c>
       <c r="R11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="S11" t="n">
         <v>0.0</v>
       </c>
       <c r="T11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U11" t="n">
         <v>0.0</v>
       </c>
       <c r="V11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12">
@@ -1536,19 +1539,19 @@
         <v>1446404.0</v>
       </c>
       <c r="C12" t="n">
-        <v>2279.0</v>
+        <v>2278.0</v>
       </c>
       <c r="D12" t="n">
-        <v>71.0</v>
+        <v>349.0</v>
       </c>
       <c r="E12" t="s">
         <v>64</v>
       </c>
       <c r="F12" t="n">
-        <v>157160.0</v>
+        <v>157177.0</v>
       </c>
       <c r="G12" t="n">
-        <v>10866.0</v>
+        <v>10867.0</v>
       </c>
       <c r="H12" t="s">
         <v>97</v>
@@ -1557,43 +1560,43 @@
         <v>802.0</v>
       </c>
       <c r="J12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K12" t="n">
         <v>27.0</v>
       </c>
       <c r="L12" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="M12" t="n">
         <v>0.0</v>
       </c>
       <c r="N12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O12" t="n">
         <v>7.0</v>
       </c>
       <c r="P12" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="Q12" t="n">
         <v>748.0</v>
       </c>
       <c r="R12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="S12" t="n">
         <v>5.0</v>
       </c>
       <c r="T12" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="U12" t="n">
         <v>15.0</v>
       </c>
       <c r="V12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13">
@@ -1613,10 +1616,10 @@
         <v>65</v>
       </c>
       <c r="F13" t="n">
-        <v>59932.0</v>
+        <v>59945.0</v>
       </c>
       <c r="G13" t="n">
-        <v>8738.0</v>
+        <v>8740.0</v>
       </c>
       <c r="H13" t="s">
         <v>97</v>
@@ -1625,43 +1628,43 @@
         <v>123.0</v>
       </c>
       <c r="J13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K13" t="n">
         <v>6.0</v>
       </c>
       <c r="L13" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="M13" t="n">
         <v>0.0</v>
       </c>
       <c r="N13" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O13" t="n">
         <v>2.0</v>
       </c>
       <c r="P13" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="Q13" t="n">
         <v>112.0</v>
       </c>
       <c r="R13" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S13" t="n">
         <v>1.0</v>
       </c>
       <c r="T13" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U13" t="n">
         <v>2.0</v>
       </c>
       <c r="V13" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14">
@@ -1672,19 +1675,19 @@
         <v>289468.0</v>
       </c>
       <c r="C14" t="n">
-        <v>516.0</v>
+        <v>515.0</v>
       </c>
       <c r="D14" t="n">
-        <v>395.0</v>
+        <v>394.0</v>
       </c>
       <c r="E14" t="s">
         <v>66</v>
       </c>
       <c r="F14" t="n">
-        <v>37856.0</v>
+        <v>37855.0</v>
       </c>
       <c r="G14" t="n">
-        <v>13078.0</v>
+        <v>13077.0</v>
       </c>
       <c r="H14" t="s">
         <v>98</v>
@@ -1693,43 +1696,43 @@
         <v>276.0</v>
       </c>
       <c r="J14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K14" t="n">
         <v>5.0</v>
       </c>
       <c r="L14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M14" t="n">
         <v>0.0</v>
       </c>
       <c r="N14" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O14" t="n">
         <v>1.0</v>
       </c>
       <c r="P14" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Q14" t="n">
         <v>268.0</v>
       </c>
       <c r="R14" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="S14" t="n">
         <v>0.0</v>
       </c>
       <c r="T14" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U14" t="n">
         <v>2.0</v>
       </c>
       <c r="V14" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15">
@@ -1749,10 +1752,10 @@
         <v>67</v>
       </c>
       <c r="F15" t="n">
-        <v>29025.0</v>
+        <v>29029.0</v>
       </c>
       <c r="G15" t="n">
-        <v>14820.0</v>
+        <v>14823.0</v>
       </c>
       <c r="H15" t="s">
         <v>99</v>
@@ -1761,43 +1764,43 @@
         <v>227.0</v>
       </c>
       <c r="J15" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K15" t="n">
         <v>7.0</v>
       </c>
       <c r="L15" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="M15" t="n">
         <v>0.0</v>
       </c>
       <c r="N15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O15" t="n">
         <v>4.0</v>
       </c>
       <c r="P15" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="Q15" t="n">
         <v>207.0</v>
       </c>
       <c r="R15" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="S15" t="n">
         <v>0.0</v>
       </c>
       <c r="T15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U15" t="n">
         <v>9.0</v>
       </c>
       <c r="V15" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="16">
@@ -1817,10 +1820,10 @@
         <v>68</v>
       </c>
       <c r="F16" t="n">
-        <v>30347.0</v>
+        <v>30348.0</v>
       </c>
       <c r="G16" t="n">
-        <v>11025.0</v>
+        <v>11026.0</v>
       </c>
       <c r="H16" t="s">
         <v>100</v>
@@ -1829,43 +1832,43 @@
         <v>176.0</v>
       </c>
       <c r="J16" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K16" t="n">
         <v>9.0</v>
       </c>
       <c r="L16" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="M16" t="n">
         <v>0.0</v>
       </c>
       <c r="N16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O16" t="n">
         <v>0.0</v>
       </c>
       <c r="P16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q16" t="n">
         <v>161.0</v>
       </c>
       <c r="R16" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="S16" t="n">
         <v>4.0</v>
       </c>
       <c r="T16" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="U16" t="n">
         <v>2.0</v>
       </c>
       <c r="V16" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17">
@@ -1879,16 +1882,16 @@
         <v>1658.0</v>
       </c>
       <c r="D17" t="n">
-        <v>91.0</v>
+        <v>448.0</v>
       </c>
       <c r="E17" t="s">
         <v>69</v>
       </c>
       <c r="F17" t="n">
-        <v>64827.0</v>
+        <v>64811.0</v>
       </c>
       <c r="G17" t="n">
-        <v>7916.0</v>
+        <v>7914.0</v>
       </c>
       <c r="H17" t="s">
         <v>101</v>
@@ -1897,43 +1900,43 @@
         <v>94.0</v>
       </c>
       <c r="J17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="K17" t="n">
         <v>13.0</v>
       </c>
       <c r="L17" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="M17" t="n">
         <v>0.0</v>
       </c>
       <c r="N17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O17" t="n">
         <v>1.0</v>
       </c>
       <c r="P17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="Q17" t="n">
         <v>79.0</v>
       </c>
       <c r="R17" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="S17" t="n">
         <v>0.0</v>
       </c>
       <c r="T17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U17" t="n">
         <v>1.0</v>
       </c>
       <c r="V17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18">
@@ -1953,10 +1956,10 @@
         <v>70</v>
       </c>
       <c r="F18" t="n">
-        <v>22097.0</v>
+        <v>22081.0</v>
       </c>
       <c r="G18" t="n">
-        <v>5349.0</v>
+        <v>5345.0</v>
       </c>
       <c r="H18" t="s">
         <v>102</v>
@@ -1965,43 +1968,43 @@
         <v>36.0</v>
       </c>
       <c r="J18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K18" t="n">
         <v>1.0</v>
       </c>
       <c r="L18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M18" t="n">
         <v>0.0</v>
       </c>
       <c r="N18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O18" t="n">
         <v>1.0</v>
       </c>
       <c r="P18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="Q18" t="n">
         <v>34.0</v>
       </c>
       <c r="R18" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="S18" t="n">
         <v>0.0</v>
       </c>
       <c r="T18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U18" t="n">
         <v>0.0</v>
       </c>
       <c r="V18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19">
@@ -2033,43 +2036,43 @@
         <v>0.0</v>
       </c>
       <c r="J19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K19" t="n">
         <v>0.0</v>
       </c>
       <c r="L19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M19" t="n">
         <v>0.0</v>
       </c>
       <c r="N19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O19" t="n">
         <v>0.0</v>
       </c>
       <c r="P19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q19" t="n">
         <v>0.0</v>
       </c>
       <c r="R19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="S19" t="n">
         <v>0.0</v>
       </c>
       <c r="T19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U19" t="n">
         <v>0.0</v>
       </c>
       <c r="V19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20">
@@ -2101,43 +2104,43 @@
         <v>3.0</v>
       </c>
       <c r="J20" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K20" t="n">
         <v>0.0</v>
       </c>
       <c r="L20" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M20" t="n">
         <v>0.0</v>
       </c>
       <c r="N20" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O20" t="n">
         <v>0.0</v>
       </c>
       <c r="P20" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q20" t="n">
         <v>3.0</v>
       </c>
       <c r="R20" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="S20" t="n">
         <v>0.0</v>
       </c>
       <c r="T20" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U20" t="n">
         <v>0.0</v>
       </c>
       <c r="V20" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21">
@@ -2148,10 +2151,10 @@
         <v>160480.0</v>
       </c>
       <c r="C21" t="n">
-        <v>371.0</v>
+        <v>372.0</v>
       </c>
       <c r="D21" t="n">
-        <v>512.0</v>
+        <v>513.0</v>
       </c>
       <c r="E21" t="s">
         <v>73</v>
@@ -2169,43 +2172,43 @@
         <v>47.0</v>
       </c>
       <c r="J21" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K21" t="n">
         <v>10.0</v>
       </c>
       <c r="L21" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M21" t="n">
         <v>0.0</v>
       </c>
       <c r="N21" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O21" t="n">
         <v>0.0</v>
       </c>
       <c r="P21" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q21" t="n">
         <v>36.0</v>
       </c>
       <c r="R21" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="S21" t="n">
         <v>0.0</v>
       </c>
       <c r="T21" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U21" t="n">
         <v>1.0</v>
       </c>
       <c r="V21" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22">
@@ -2237,43 +2240,43 @@
         <v>0.0</v>
       </c>
       <c r="J22" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K22" t="n">
         <v>0.0</v>
       </c>
       <c r="L22" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M22" t="n">
         <v>0.0</v>
       </c>
       <c r="N22" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O22" t="n">
         <v>0.0</v>
       </c>
       <c r="P22" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q22" t="n">
         <v>0.0</v>
       </c>
       <c r="R22" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="S22" t="n">
         <v>0.0</v>
       </c>
       <c r="T22" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U22" t="n">
         <v>0.0</v>
       </c>
       <c r="V22" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23">
@@ -2284,10 +2287,10 @@
         <v>127642.0</v>
       </c>
       <c r="C23" t="n">
-        <v>327.0</v>
+        <v>326.0</v>
       </c>
       <c r="D23" t="n">
-        <v>567.0</v>
+        <v>566.0</v>
       </c>
       <c r="E23" t="s">
         <v>75</v>
@@ -2305,43 +2308,43 @@
         <v>8.0</v>
       </c>
       <c r="J23" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K23" t="n">
         <v>2.0</v>
       </c>
       <c r="L23" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="M23" t="n">
         <v>0.0</v>
       </c>
       <c r="N23" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O23" t="n">
         <v>0.0</v>
       </c>
       <c r="P23" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q23" t="n">
         <v>6.0</v>
       </c>
       <c r="R23" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="S23" t="n">
         <v>0.0</v>
       </c>
       <c r="T23" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U23" t="n">
         <v>0.0</v>
       </c>
       <c r="V23" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24">
@@ -2355,16 +2358,16 @@
         <v>4812.0</v>
       </c>
       <c r="D24" t="n">
-        <v>86.0</v>
+        <v>422.0</v>
       </c>
       <c r="E24" t="s">
         <v>76</v>
       </c>
       <c r="F24" t="n">
-        <v>198729.0</v>
+        <v>198523.0</v>
       </c>
       <c r="G24" t="n">
-        <v>7873.0</v>
+        <v>7865.0</v>
       </c>
       <c r="H24" t="s">
         <v>108</v>
@@ -2373,43 +2376,43 @@
         <v>819.0</v>
       </c>
       <c r="J24" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K24" t="n">
         <v>19.0</v>
       </c>
       <c r="L24" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="M24" t="n">
         <v>1.0</v>
       </c>
       <c r="N24" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="O24" t="n">
         <v>5.0</v>
       </c>
       <c r="P24" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="Q24" t="n">
         <v>780.0</v>
       </c>
       <c r="R24" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="S24" t="n">
         <v>1.0</v>
       </c>
       <c r="T24" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="U24" t="n">
         <v>13.0</v>
       </c>
       <c r="V24" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="25">
@@ -2441,43 +2444,43 @@
         <v>0.0</v>
       </c>
       <c r="J25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K25" t="n">
         <v>0.0</v>
       </c>
       <c r="L25" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M25" t="n">
         <v>0.0</v>
       </c>
       <c r="N25" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O25" t="n">
         <v>0.0</v>
       </c>
       <c r="P25" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q25" t="n">
         <v>0.0</v>
       </c>
       <c r="R25" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="S25" t="n">
         <v>0.0</v>
       </c>
       <c r="T25" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U25" t="n">
         <v>0.0</v>
       </c>
       <c r="V25" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26">
@@ -2497,10 +2500,10 @@
         <v>78</v>
       </c>
       <c r="F26" t="n">
-        <v>3174.0</v>
+        <v>3175.0</v>
       </c>
       <c r="G26" t="n">
-        <v>5725.0</v>
+        <v>5726.0</v>
       </c>
       <c r="H26" t="s">
         <v>110</v>
@@ -2509,43 +2512,43 @@
         <v>0.0</v>
       </c>
       <c r="J26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K26" t="n">
         <v>0.0</v>
       </c>
       <c r="L26" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M26" t="n">
         <v>0.0</v>
       </c>
       <c r="N26" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O26" t="n">
         <v>0.0</v>
       </c>
       <c r="P26" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q26" t="n">
         <v>0.0</v>
       </c>
       <c r="R26" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="S26" t="n">
         <v>0.0</v>
       </c>
       <c r="T26" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U26" t="n">
         <v>0.0</v>
       </c>
       <c r="V26" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27">
@@ -2577,43 +2580,43 @@
         <v>1.0</v>
       </c>
       <c r="J27" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="K27" t="n">
         <v>0.0</v>
       </c>
       <c r="L27" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M27" t="n">
         <v>0.0</v>
       </c>
       <c r="N27" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O27" t="n">
         <v>0.0</v>
       </c>
       <c r="P27" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q27" t="n">
         <v>1.0</v>
       </c>
       <c r="R27" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="S27" t="n">
         <v>0.0</v>
       </c>
       <c r="T27" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U27" t="n">
         <v>0.0</v>
       </c>
       <c r="V27" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28">
@@ -2633,55 +2636,55 @@
         <v>80</v>
       </c>
       <c r="F28" t="n">
-        <v>31143.0</v>
+        <v>31141.0</v>
       </c>
       <c r="G28" t="n">
-        <v>6098.0</v>
+        <v>6097.0</v>
       </c>
       <c r="H28" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="I28" t="n">
         <v>55.0</v>
       </c>
       <c r="J28" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K28" t="n">
         <v>2.0</v>
       </c>
       <c r="L28" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="M28" t="n">
         <v>1.0</v>
       </c>
       <c r="N28" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="O28" t="n">
         <v>0.0</v>
       </c>
       <c r="P28" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q28" t="n">
         <v>52.0</v>
       </c>
       <c r="R28" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="S28" t="n">
         <v>0.0</v>
       </c>
       <c r="T28" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U28" t="n">
         <v>0.0</v>
       </c>
       <c r="V28" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29">
@@ -2701,55 +2704,55 @@
         <v>81</v>
       </c>
       <c r="F29" t="n">
-        <v>5818.0</v>
+        <v>5816.0</v>
       </c>
       <c r="G29" t="n">
-        <v>7065.0</v>
+        <v>7063.0</v>
       </c>
       <c r="H29" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I29" t="n">
         <v>54.0</v>
       </c>
       <c r="J29" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K29" t="n">
         <v>2.0</v>
       </c>
       <c r="L29" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="M29" t="n">
         <v>0.0</v>
       </c>
       <c r="N29" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O29" t="n">
         <v>2.0</v>
       </c>
       <c r="P29" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="Q29" t="n">
         <v>50.0</v>
       </c>
       <c r="R29" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="S29" t="n">
         <v>0.0</v>
       </c>
       <c r="T29" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U29" t="n">
         <v>0.0</v>
       </c>
       <c r="V29" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30">
@@ -2775,49 +2778,49 @@
         <v>5416.0</v>
       </c>
       <c r="H30" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I30" t="n">
         <v>24.0</v>
       </c>
       <c r="J30" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K30" t="n">
         <v>2.0</v>
       </c>
       <c r="L30" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="M30" t="n">
         <v>0.0</v>
       </c>
       <c r="N30" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O30" t="n">
         <v>0.0</v>
       </c>
       <c r="P30" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q30" t="n">
         <v>22.0</v>
       </c>
       <c r="R30" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="S30" t="n">
         <v>0.0</v>
       </c>
       <c r="T30" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U30" t="n">
         <v>0.0</v>
       </c>
       <c r="V30" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31">
@@ -2837,55 +2840,55 @@
         <v>83</v>
       </c>
       <c r="F31" t="n">
-        <v>138842.0</v>
+        <v>138639.0</v>
       </c>
       <c r="G31" t="n">
-        <v>9020.0</v>
+        <v>9007.0</v>
       </c>
       <c r="H31" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I31" t="n">
         <v>685.0</v>
       </c>
       <c r="J31" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K31" t="n">
         <v>13.0</v>
       </c>
       <c r="L31" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="M31" t="n">
         <v>0.0</v>
       </c>
       <c r="N31" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O31" t="n">
         <v>3.0</v>
       </c>
       <c r="P31" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Q31" t="n">
         <v>655.0</v>
       </c>
       <c r="R31" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="S31" t="n">
         <v>1.0</v>
       </c>
       <c r="T31" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="U31" t="n">
         <v>13.0</v>
       </c>
       <c r="V31" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32">
@@ -2896,64 +2899,64 @@
         <v>550512.0</v>
       </c>
       <c r="C32" t="n">
-        <v>1008.0</v>
+        <v>1009.0</v>
       </c>
       <c r="D32" t="n">
-        <v>83.0</v>
+        <v>406.0</v>
       </c>
       <c r="E32" t="s">
         <v>84</v>
       </c>
       <c r="F32" t="n">
-        <v>29546.0</v>
+        <v>29548.0</v>
       </c>
       <c r="G32" t="n">
         <v>5367.0</v>
       </c>
       <c r="H32" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I32" t="n">
         <v>272.0</v>
       </c>
       <c r="J32" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="K32" t="n">
         <v>10.0</v>
       </c>
       <c r="L32" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="M32" t="n">
         <v>0.0</v>
       </c>
       <c r="N32" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O32" t="n">
         <v>1.0</v>
       </c>
       <c r="P32" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Q32" t="n">
         <v>248.0</v>
       </c>
       <c r="R32" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="S32" t="n">
         <v>1.0</v>
       </c>
       <c r="T32" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U32" t="n">
         <v>12.0</v>
       </c>
       <c r="V32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="33">
@@ -2979,49 +2982,49 @@
         <v>5755.0</v>
       </c>
       <c r="H33" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I33" t="n">
         <v>43.0</v>
       </c>
       <c r="J33" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K33" t="n">
         <v>3.0</v>
       </c>
       <c r="L33" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="M33" t="n">
         <v>0.0</v>
       </c>
       <c r="N33" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O33" t="n">
         <v>0.0</v>
       </c>
       <c r="P33" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q33" t="n">
         <v>40.0</v>
       </c>
       <c r="R33" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="S33" t="n">
         <v>0.0</v>
       </c>
       <c r="T33" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U33" t="n">
         <v>0.0</v>
       </c>
       <c r="V33" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34">
@@ -3032,64 +3035,64 @@
         <v>351491.0</v>
       </c>
       <c r="C34" t="n">
-        <v>659.0</v>
+        <v>660.0</v>
       </c>
       <c r="D34" t="n">
-        <v>415.0</v>
+        <v>416.0</v>
       </c>
       <c r="E34" t="s">
         <v>86</v>
       </c>
       <c r="F34" t="n">
-        <v>18093.0</v>
+        <v>18095.0</v>
       </c>
       <c r="G34" t="n">
         <v>5148.0</v>
       </c>
       <c r="H34" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I34" t="n">
         <v>229.0</v>
       </c>
       <c r="J34" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K34" t="n">
         <v>7.0</v>
       </c>
       <c r="L34" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="M34" t="n">
         <v>0.0</v>
       </c>
       <c r="N34" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O34" t="n">
         <v>1.0</v>
       </c>
       <c r="P34" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="Q34" t="n">
         <v>208.0</v>
       </c>
       <c r="R34" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="S34" t="n">
         <v>1.0</v>
       </c>
       <c r="T34" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="U34" t="n">
         <v>12.0</v>
       </c>
       <c r="V34" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>